<commit_message>
Did the normal form process diagrams for the database structure
</commit_message>
<xml_diff>
--- a/assessment1/spreadsheets/ARA DATA Wait Lists Feb 2021.xlsx
+++ b/assessment1/spreadsheets/ARA DATA Wait Lists Feb 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finle\Documents\DE103\assessment1\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE61D436-0FC8-4639-B1A1-7F38F8F5A1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4413636C-CB42-48DE-9F13-D1525D2F056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31170" yWindow="7740" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleansed Data" sheetId="1" r:id="rId1"/>
@@ -3256,8 +3256,8 @@
   <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25911,7 +25911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28200,9 +28200,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370288AA-62BE-4E42-95A9-B994B0507A38}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30979,7 +30979,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31022,7 +31022,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31100,7 +31100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4844EEF0-6272-426F-89E2-272D365FCB0F}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished on the design issues and version control report.
</commit_message>
<xml_diff>
--- a/assessment1/spreadsheets/ARA DATA Wait Lists Feb 2021.xlsx
+++ b/assessment1/spreadsheets/ARA DATA Wait Lists Feb 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finle\Documents\DE103\assessment1\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4413636C-CB42-48DE-9F13-D1525D2F056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB7F2B9-D8D4-439B-BD6C-CF2015A00B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31170" yWindow="7740" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleansed Data" sheetId="1" r:id="rId1"/>
@@ -2866,7 +2866,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3256,7 +3286,7 @@
   <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
@@ -7231,13 +7261,13 @@
     <sortCondition ref="L2:L94"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"MFO6152"</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Plastics"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27894,16 +27924,16 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="7" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
       <formula>"MFO6152"</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="5" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="4" priority="19" operator="containsText" text="YBB">
+    <cfRule type="containsText" dxfId="7" priority="19" operator="containsText" text="YBB">
       <formula>NOT(ISERROR(SEARCH("YBB",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28200,7 +28230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370288AA-62BE-4E42-95A9-B994B0507A38}">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
@@ -30771,7 +30801,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Richards">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Richards">
       <formula>NOT(ISERROR(SEARCH("Richards",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31100,7 +31130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4844EEF0-6272-426F-89E2-272D365FCB0F}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -32995,7 +33025,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -33007,7 +33037,7 @@
   <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37463,12 +37493,13 @@
     <sortCondition ref="K2:K101"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="YBB">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="YBB">
       <formula>NOT(ISERROR(SEARCH("YBB",E1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"YBB"</formula>
     </cfRule>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>